<commit_message>
envoi de quelques documents
</commit_message>
<xml_diff>
--- a/DUCMA_documents/estimation.xlsx
+++ b/DUCMA_documents/estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -138,6 +138,27 @@
   </si>
   <si>
     <t>faire en sorte que le serveur ne soit pas seulement en local</t>
+  </si>
+  <si>
+    <t>commencer les  activity et le java</t>
+  </si>
+  <si>
+    <t>mise en place du serveur apache, php, mysql et phpmyadmin</t>
+  </si>
+  <si>
+    <t>création de la bd</t>
+  </si>
+  <si>
+    <t>tentative de connexion à la bd (échec)</t>
+  </si>
+  <si>
+    <t>documentation</t>
+  </si>
+  <si>
+    <t>tentative de requête à l'aide d'android(échec)</t>
+  </si>
+  <si>
+    <t>documentation concernant android et php</t>
   </si>
 </sst>
 </file>
@@ -281,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -318,6 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1589,7 +1611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -1698,10 +1720,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="11">
         <f>SUM(C16:C20)</f>
         <v>82</v>
@@ -1791,10 +1813,10 @@
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="19"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="11">
         <f>SUM(C26:C33)</f>
         <v>8</v>
@@ -1821,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD47"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1879,44 +1901,92 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12">
+        <v>42765</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="18">
+        <v>42766</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="18">
+        <v>42772</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="18">
+        <v>42773</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="18">
+        <v>42775</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
+      <c r="A19" s="18">
+        <v>42779</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
+      <c r="A20" s="18">
+        <v>42780</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="15">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
+      <c r="A21" s="18">
+        <v>42783</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
@@ -1994,13 +2064,13 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2022,22 +2092,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="20"/>
+      <c r="B42" s="21"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="21"/>
+      <c r="B43" s="22"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="21"/>
+      <c r="B44" s="22"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="21"/>
+      <c r="B45" s="22"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="21"/>
+      <c r="B46" s="22"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="22"/>
+      <c r="B47" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2229,10 +2299,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2257,22 +2327,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="20"/>
+      <c r="B42" s="21"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="21"/>
+      <c r="B43" s="22"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="21"/>
+      <c r="B44" s="22"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="21"/>
+      <c r="B45" s="22"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="21"/>
+      <c r="B46" s="22"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="22"/>
+      <c r="B47" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2462,10 +2532,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2490,22 +2560,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="20"/>
+      <c r="B42" s="21"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="21"/>
+      <c r="B43" s="22"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="21"/>
+      <c r="B44" s="22"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="21"/>
+      <c r="B45" s="22"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="21"/>
+      <c r="B46" s="22"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="22"/>
+      <c r="B47" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2695,10 +2765,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2723,22 +2793,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="20"/>
+      <c r="B42" s="21"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="21"/>
+      <c r="B43" s="22"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="21"/>
+      <c r="B44" s="22"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="21"/>
+      <c r="B45" s="22"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="21"/>
+      <c r="B46" s="22"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="22"/>
+      <c r="B47" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>